<commit_message>
reasoning transfer - COG
Signed-off-by: ibm <tkornuta.ibm@gmail.com>
</commit_message>
<xml_diff>
--- a/Transfer_Learning/results/reasoning_transfer_COG_RESULTS.xlsx
+++ b/Transfer_Learning/results/reasoning_transfer_COG_RESULTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkornuta/Documents/git/mi-visual-reasoning-pubs/Transfer_Learning/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC28663-CD96-AA41-A011-257196CD0095}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDF861F-AC2F-0240-BD86-9AE8EF1960F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2900" yWindow="460" windowWidth="21980" windowHeight="14460" activeTab="1" xr2:uid="{4BA6BB31-2F0E-4947-A980-9A98EA29CC77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
   <si>
     <t>AndCompareColor</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Group A/B Training</t>
+  </si>
+  <si>
+    <t>Train on All</t>
+  </si>
+  <si>
+    <t>Train on t only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train on Group A/B </t>
   </si>
 </sst>
 </file>
@@ -360,9 +369,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -394,6 +400,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1722,15 +1731,15 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>barcharts!$B$36</c:f>
+              <c:f>barcharts!$D$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Single-task training</c:v>
+                  <c:v>Train on All</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1746,102 +1755,6 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="1.5162885812716919E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-57F0-974E-A8F3-4AB2D00FB62D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.7957372711402864E-3"/>
-                  <c:y val="1.8246548282526743E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-57F0-974E-A8F3-4AB2D00FB62D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1921,6 +1834,192 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:f>barcharts!$D$37:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.99985214889999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97033816616666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99591481312499996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95671318045999987</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98294628853333332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8A8D-0D4B-8EB9-992912EC0F6D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>barcharts!$B$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Train on t only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.5162885812716919E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-57F0-974E-A8F3-4AB2D00FB62D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.7957372711402864E-3"/>
+                  <c:y val="1.8246548282526743E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-57F0-974E-A8F3-4AB2D00FB62D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>barcharts!$A$37:$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Basic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compare</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Obj-Attr</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cognitive</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Spatial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>barcharts!$B$37:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
@@ -1951,14 +2050,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>barcharts!$C$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Group A/B Training</c:v>
+                  <c:v>Train on Group A/B </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2089,151 +2188,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8A8D-0D4B-8EB9-992912EC0F6D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>barcharts!$D$36</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>All-tasks training</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="pct5">
-              <a:fgClr>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>barcharts!$A$37:$A$41</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Basic</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Compare</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Obj-Attr</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Cognitive</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Spatial</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>barcharts!$D$37:$D$41</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.99985214889999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.97033816616666668</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.99591481312499996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.95671318045999987</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.98294628853333332</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8A8D-0D4B-8EB9-992912EC0F6D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4494,11 +4448,11 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="str">
+      <c r="A2" s="18" t="str">
         <f>"Compare + Basic: "&amp;ROUND(AVERAGE(C2:C16) * 100, 2)&amp; "%"</f>
         <v>Compare + Basic: 96.67%</v>
       </c>
-      <c r="B2" s="21" t="str">
+      <c r="B2" s="20" t="str">
         <f>"Basic: "&amp;ROUND(AVERAGE(C2:C6) * 100, 1)&amp; "%"</f>
         <v>Basic: 100%</v>
       </c>
@@ -4506,10 +4460,10 @@
         <v>0.99980200630000005</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="27">
         <v>1</v>
       </c>
       <c r="G2" s="3"/>
@@ -4519,11 +4473,11 @@
       <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="28">
         <f>AVERAGE(I2:I6)</f>
         <v>0.99985214889999996</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="17" t="s">
         <v>25</v>
       </c>
       <c r="M2" t="s">
@@ -4531,14 +4485,14 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="6">
         <v>0.99997800069999998</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="28"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="3"/>
       <c r="H3" t="s">
         <v>19</v>
@@ -4546,21 +4500,21 @@
       <c r="I3" s="2">
         <v>0.99990595540000005</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="L3" s="18"/>
+      <c r="J3" s="17"/>
+      <c r="L3" s="17"/>
       <c r="M3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="6">
         <v>0.99975800770000001</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="28"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="3"/>
       <c r="H4" t="s">
         <v>17</v>
@@ -4568,21 +4522,21 @@
       <c r="I4" s="2">
         <v>0.99988277219999999</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="J4" s="17"/>
+      <c r="L4" s="17"/>
       <c r="M4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="6">
         <v>0.99962382149999995</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="28"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="3"/>
       <c r="H5" t="s">
         <v>7</v>
@@ -4590,21 +4544,21 @@
       <c r="I5" s="2">
         <v>0.99975800770000001</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="L5" s="18"/>
+      <c r="J5" s="17"/>
+      <c r="L5" s="17"/>
       <c r="M5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="8">
         <v>0.99974209879999998</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="28"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="3"/>
       <c r="H6" t="s">
         <v>6</v>
@@ -4612,8 +4566,8 @@
       <c r="I6" s="2">
         <v>0.99971400919999998</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="L6" s="18" t="s">
+      <c r="J6" s="17"/>
+      <c r="L6" s="17" t="s">
         <v>6</v>
       </c>
       <c r="M6" t="s">
@@ -4621,8 +4575,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="24" t="str">
+      <c r="A7" s="18"/>
+      <c r="B7" s="23" t="str">
         <f>"Compare 2 Objects: "&amp;ROUND(AVERAGE(C7:C12) * 100, 1)&amp; "%"</f>
         <v>Compare 2 Objects: 92.3%</v>
       </c>
@@ -4630,10 +4584,10 @@
         <v>0.99842408559999996</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="27">
         <v>0.58589999999999998</v>
       </c>
       <c r="G7" s="3"/>
@@ -4643,24 +4597,24 @@
       <c r="I7" s="2">
         <v>0.99945901449999996</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="28">
         <f>AVERAGE(I7:I12)</f>
         <v>0.97033816616666668</v>
       </c>
-      <c r="L7" s="18"/>
+      <c r="L7" s="17"/>
       <c r="M7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="6">
         <v>0.99195256249999997</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="28"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="3"/>
       <c r="H8" t="s">
         <v>14</v>
@@ -4668,21 +4622,21 @@
       <c r="I8" s="2">
         <v>0.99402324819999999</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="L8" s="18"/>
+      <c r="J8" s="28"/>
+      <c r="L8" s="17"/>
       <c r="M8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="6">
         <v>0.97622512149999996</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="28"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="3"/>
       <c r="H9" t="s">
         <v>4</v>
@@ -4690,21 +4644,21 @@
       <c r="I9" s="2">
         <v>0.98118233160000001</v>
       </c>
-      <c r="J9" s="17"/>
-      <c r="L9" s="18"/>
+      <c r="J9" s="28"/>
+      <c r="L9" s="17"/>
       <c r="M9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="6">
         <v>0.97538811989999996</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="28"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3"/>
       <c r="H10" t="s">
         <v>5</v>
@@ -4712,21 +4666,21 @@
       <c r="I10" s="2">
         <v>0.9804640107</v>
       </c>
-      <c r="J10" s="17"/>
-      <c r="L10" s="18"/>
+      <c r="J10" s="28"/>
+      <c r="L10" s="17"/>
       <c r="M10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="6">
         <v>0.79776099469999995</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="28"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3"/>
       <c r="H11" t="s">
         <v>0</v>
@@ -4734,21 +4688,21 @@
       <c r="I11" s="2">
         <v>0.93489399939999995</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="L11" s="18"/>
+      <c r="J11" s="28"/>
+      <c r="L11" s="17"/>
       <c r="M11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="8">
         <v>0.79534117869999998</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="28"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="3"/>
       <c r="H12" t="s">
         <v>1</v>
@@ -4756,15 +4710,15 @@
       <c r="I12" s="2">
         <v>0.93200639259999996</v>
       </c>
-      <c r="J12" s="17"/>
-      <c r="L12" s="18"/>
+      <c r="J12" s="28"/>
+      <c r="L12" s="17"/>
       <c r="M12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="24" t="str">
+      <c r="A13" s="18"/>
+      <c r="B13" s="23" t="str">
         <f>"Compare Obj Attr: "&amp;ROUND(AVERAGE(C13:C16) * 100, 1)&amp; "%"</f>
         <v>Compare Obj Attr: 99.2%</v>
       </c>
@@ -4772,10 +4726,10 @@
         <v>0.99922642350000002</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="27">
         <v>0.99680000000000002</v>
       </c>
       <c r="G13" s="3"/>
@@ -4785,24 +4739,24 @@
       <c r="I13" s="2">
         <v>0.99981246629999998</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="28">
         <f>AVERAGE(I13:I16)</f>
         <v>0.99591481312499996</v>
       </c>
-      <c r="L13" s="18"/>
+      <c r="L13" s="17"/>
       <c r="M13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="6">
         <v>0.99906052560000003</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="28"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="3"/>
       <c r="H14" t="s">
         <v>21</v>
@@ -4810,21 +4764,21 @@
       <c r="I14" s="2">
         <v>0.99938934170000004</v>
       </c>
-      <c r="J14" s="18"/>
-      <c r="L14" s="18"/>
+      <c r="J14" s="17"/>
+      <c r="L14" s="17"/>
       <c r="M14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="6">
         <v>0.98497561430000002</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="28"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="3"/>
       <c r="H15" t="s">
         <v>3</v>
@@ -4832,21 +4786,21 @@
       <c r="I15" s="2">
         <v>0.99248780709999995</v>
       </c>
-      <c r="J15" s="18"/>
-      <c r="L15" s="18"/>
+      <c r="J15" s="17"/>
+      <c r="L15" s="17"/>
       <c r="M15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="8">
         <v>0.98398555919999997</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="28"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="3"/>
       <c r="H16" t="s">
         <v>2</v>
@@ -4854,18 +4808,18 @@
       <c r="I16" s="2">
         <v>0.99196963739999999</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="L16" s="18"/>
+      <c r="J16" s="17"/>
+      <c r="L16" s="17"/>
       <c r="M16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="str">
+      <c r="A17" s="26" t="str">
         <f>"Spatial + Cognitive: "&amp;ROUND(AVERAGE(C17:C24) * 100, 2)&amp; "%"</f>
         <v>Spatial + Cognitive: 96.68%</v>
       </c>
-      <c r="B17" s="24" t="str">
+      <c r="B17" s="23" t="str">
         <f>"Spatial: "&amp;ROUND(AVERAGE(C17:C21) * 100, 1)&amp; "%"</f>
         <v>Spatial: 96.4%</v>
       </c>
@@ -4873,10 +4827,10 @@
         <v>0.96315356600000002</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="27">
         <v>0.96679999999999999</v>
       </c>
       <c r="G17" s="3"/>
@@ -4886,11 +4840,11 @@
       <c r="I17" s="2">
         <v>0.95311949240000005</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="28">
         <f>AVERAGE(I17:I21)</f>
         <v>0.95671318045999987</v>
       </c>
-      <c r="L17" s="18" t="s">
+      <c r="L17" s="17" t="s">
         <v>30</v>
       </c>
       <c r="M17" t="s">
@@ -4898,14 +4852,14 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="9">
         <v>0.95398338680000005</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="28"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="27"/>
       <c r="G18" s="3"/>
       <c r="H18" t="s">
         <v>9</v>
@@ -4913,21 +4867,21 @@
       <c r="I18" s="2">
         <v>0.94067396640000001</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="L18" s="18"/>
+      <c r="J18" s="17"/>
+      <c r="L18" s="17"/>
       <c r="M18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="6">
         <v>0.94789975289999995</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="28"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="27"/>
       <c r="G19" s="3"/>
       <c r="H19" t="s">
         <v>15</v>
@@ -4935,21 +4889,21 @@
       <c r="I19" s="2">
         <v>0.93500411809999995</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="J19" s="17"/>
+      <c r="L19" s="17"/>
       <c r="M19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="9">
         <v>0.97951672670000001</v>
       </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="28"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="3"/>
       <c r="H20" t="s">
         <v>18</v>
@@ -4957,21 +4911,21 @@
       <c r="I20" s="2">
         <v>0.97992283869999997</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="L20" s="18"/>
+      <c r="J20" s="17"/>
+      <c r="L20" s="17"/>
       <c r="M20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="9">
         <v>0.97677849279999995</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="28"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="3"/>
       <c r="H21" t="s">
         <v>20</v>
@@ -4979,8 +4933,8 @@
       <c r="I21" s="2">
         <v>0.97484548670000004</v>
       </c>
-      <c r="J21" s="18"/>
-      <c r="L21" s="18" t="s">
+      <c r="J21" s="17"/>
+      <c r="L21" s="17" t="s">
         <v>31</v>
       </c>
       <c r="M21" t="s">
@@ -4988,8 +4942,8 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="25" t="str">
+      <c r="A22" s="18"/>
+      <c r="B22" s="24" t="str">
         <f>"Cognitive: "&amp;ROUND(AVERAGE(C22:C24) * 100, 1)&amp; "%"</f>
         <v>Cognitive: 97.1%</v>
       </c>
@@ -4997,10 +4951,10 @@
         <v>0.96339317140000003</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="27">
         <v>0.68559999999999999</v>
       </c>
       <c r="G22" s="3"/>
@@ -5010,24 +4964,24 @@
       <c r="I22" s="2">
         <v>0.9945441746</v>
       </c>
-      <c r="J22" s="17">
+      <c r="J22" s="28">
         <f>AVERAGE(I22:I24)</f>
         <v>0.98294628853333332</v>
       </c>
-      <c r="L22" s="18"/>
+      <c r="L22" s="17"/>
       <c r="M22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="6">
         <v>0.97386483629999998</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="28"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="27"/>
       <c r="G23" s="3"/>
       <c r="H23" t="s">
         <v>12</v>
@@ -5035,21 +4989,21 @@
       <c r="I23" s="2">
         <v>0.98160858849999999</v>
       </c>
-      <c r="J23" s="18"/>
-      <c r="L23" s="18"/>
+      <c r="J23" s="17"/>
+      <c r="L23" s="17"/>
       <c r="M23" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="8">
         <v>0.9755873196</v>
       </c>
       <c r="D24" s="3"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="28"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="27"/>
       <c r="G24" s="3"/>
       <c r="H24" t="s">
         <v>11</v>
@@ -5057,8 +5011,8 @@
       <c r="I24" s="2">
         <v>0.97268610249999998</v>
       </c>
-      <c r="J24" s="18"/>
-      <c r="L24" s="18"/>
+      <c r="J24" s="17"/>
+      <c r="L24" s="17"/>
       <c r="M24" t="s">
         <v>3</v>
       </c>
@@ -5088,6 +5042,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="J7:J12"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="E17:E21"/>
     <mergeCell ref="L21:L24"/>
     <mergeCell ref="L17:L20"/>
     <mergeCell ref="L6:L16"/>
@@ -5104,16 +5068,6 @@
     <mergeCell ref="F7:F12"/>
     <mergeCell ref="F13:F16"/>
     <mergeCell ref="F17:F21"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="E17:E21"/>
-    <mergeCell ref="J7:J12"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="J22:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5127,8 +5081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47349DBF-8E4A-314D-8482-46100F956523}">
   <dimension ref="A3:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -5385,13 +5339,13 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36"/>
       <c r="B36" s="15" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E36"/>
       <c r="F36"/>

</xml_diff>